<commit_message>
basic class working properly
</commit_message>
<xml_diff>
--- a/data/seera_analysis.xlsx
+++ b/data/seera_analysis.xlsx
@@ -498,24 +498,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -527,15 +527,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -618,92 +622,91 @@
   </sheetPr>
   <dimension ref="A1:BO122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E76" activeCellId="0" sqref="E76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="46.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="20.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="28.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="26.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="24.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="21.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="17.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="18.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="1" width="22.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="1" width="26.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="26.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="1" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="16.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="71" style="1" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="1" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="1" width="26.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="1" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="1" width="26.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="1" width="22.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="78" style="1" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="28.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="24.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="23.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="21.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="0" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="0" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="18.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="0" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="0" width="16.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="71" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="0" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="0" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="0" width="22.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -736,30 +739,30 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="0"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="BO2" s="6"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="L3" s="7"/>
+      <c r="F3" s="0"/>
+      <c r="L3" s="8"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
@@ -781,123 +784,123 @@
       <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="L4" s="7"/>
+      <c r="F4" s="0"/>
+      <c r="L4" s="8"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
       <c r="BO4" s="6"/>
     </row>
     <row r="5" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="L5" s="7"/>
+      <c r="F5" s="0"/>
+      <c r="L5" s="8"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
       <c r="BO5" s="6"/>
     </row>
     <row r="6" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="L6" s="7"/>
+      <c r="F6" s="0"/>
+      <c r="L6" s="8"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
       <c r="BO6" s="6"/>
     </row>
     <row r="7" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="L7" s="7"/>
+      <c r="F7" s="0"/>
+      <c r="L7" s="8"/>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
       <c r="BO7" s="6"/>
     </row>
     <row r="8" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="L8" s="7"/>
+      <c r="F8" s="0"/>
+      <c r="L8" s="8"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
       <c r="BO8" s="6"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="L9" s="7"/>
+      <c r="F9" s="0"/>
+      <c r="L9" s="8"/>
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
@@ -919,138 +922,139 @@
       <c r="E10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="L10" s="7"/>
+      <c r="F10" s="0"/>
+      <c r="L10" s="8"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="BO10" s="6"/>
     </row>
     <row r="11" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="L11" s="7"/>
+      <c r="F11" s="0"/>
+      <c r="L11" s="8"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
       <c r="BO11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L12" s="7"/>
+      <c r="L12" s="8"/>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
       <c r="BO12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="7"/>
+      <c r="L13" s="8"/>
       <c r="AG13" s="6"/>
       <c r="AH13" s="6"/>
       <c r="AI13" s="6"/>
       <c r="BO13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="7"/>
+      <c r="L14" s="8"/>
       <c r="AG14" s="6"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
       <c r="BO14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="C15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="7"/>
+      <c r="L15" s="8"/>
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="BO15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="L16" s="8"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
@@ -1072,7 +1076,7 @@
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="8"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
@@ -1094,73 +1098,73 @@
       <c r="E18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="7"/>
+      <c r="L18" s="8"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
       <c r="BO18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="7"/>
+      <c r="L19" s="8"/>
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
       <c r="BO19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="C20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L20" s="7"/>
+      <c r="L20" s="8"/>
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="BO20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="C21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L21" s="7"/>
+      <c r="L21" s="8"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -1182,117 +1186,117 @@
       <c r="E22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="7"/>
+      <c r="L22" s="8"/>
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="BO22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="C23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L23" s="7"/>
+      <c r="L23" s="8"/>
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="BO23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="C24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L24" s="7"/>
+      <c r="L24" s="8"/>
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
       <c r="AI24" s="6"/>
       <c r="BO24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="C25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L25" s="7"/>
+      <c r="L25" s="8"/>
       <c r="AG25" s="6"/>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="BO25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L26" s="7"/>
+      <c r="L26" s="8"/>
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
       <c r="BO26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="C27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="7"/>
+      <c r="L27" s="8"/>
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -1314,105 +1318,109 @@
       <c r="E28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L28" s="7"/>
+      <c r="L28" s="8"/>
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
       <c r="BO28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L29" s="7"/>
+      <c r="C29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="L29" s="8"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
       <c r="BO29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="C30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L30" s="7"/>
+      <c r="L30" s="8"/>
       <c r="AG30" s="6"/>
       <c r="AH30" s="6"/>
       <c r="AI30" s="6"/>
       <c r="BO30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L31" s="7"/>
+      <c r="D31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="L31" s="8"/>
       <c r="AG31" s="6"/>
       <c r="AH31" s="6"/>
       <c r="AI31" s="6"/>
       <c r="BO31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" s="7"/>
+      <c r="C32" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="L32" s="8"/>
       <c r="AG32" s="6"/>
       <c r="AH32" s="6"/>
       <c r="AI32" s="6"/>
       <c r="BO32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L33" s="7"/>
+      <c r="C33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="L33" s="8"/>
       <c r="AG33" s="6"/>
       <c r="AH33" s="6"/>
       <c r="AI33" s="6"/>
@@ -1434,291 +1442,299 @@
       <c r="E34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L34" s="7"/>
+      <c r="L34" s="8"/>
       <c r="AG34" s="6"/>
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
       <c r="BO34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="L35" s="8"/>
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
       <c r="AI35" s="6"/>
       <c r="BO35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="C36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L36" s="7"/>
+      <c r="L36" s="8"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6"/>
       <c r="AI36" s="6"/>
       <c r="BO36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="C37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L37" s="7"/>
+      <c r="L37" s="8"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="6"/>
       <c r="AI37" s="6"/>
       <c r="BO37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="D38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L38" s="7"/>
+      <c r="L38" s="8"/>
       <c r="AG38" s="6"/>
       <c r="AH38" s="6"/>
       <c r="AI38" s="6"/>
       <c r="BO38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="C39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L39" s="7"/>
+      <c r="L39" s="8"/>
       <c r="AG39" s="6"/>
       <c r="AH39" s="6"/>
       <c r="AI39" s="6"/>
       <c r="BO39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="C40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L40" s="7"/>
+      <c r="L40" s="8"/>
       <c r="AG40" s="6"/>
       <c r="AH40" s="6"/>
       <c r="AI40" s="6"/>
       <c r="BO40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="C41" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L41" s="7"/>
+      <c r="L41" s="8"/>
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
       <c r="AI41" s="6"/>
       <c r="BO41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="L42" s="8"/>
       <c r="AG42" s="6"/>
       <c r="AH42" s="6"/>
       <c r="AI42" s="6"/>
       <c r="BO42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="L43" s="8"/>
       <c r="AG43" s="6"/>
       <c r="AH43" s="6"/>
       <c r="AI43" s="6"/>
       <c r="BO43" s="6"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="L44" s="8"/>
       <c r="AG44" s="6"/>
       <c r="AH44" s="6"/>
       <c r="AI44" s="6"/>
       <c r="BO44" s="6"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="L45" s="8"/>
       <c r="AG45" s="6"/>
       <c r="AH45" s="6"/>
       <c r="AI45" s="6"/>
       <c r="BO45" s="6"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="L46" s="8"/>
       <c r="AG46" s="6"/>
       <c r="AH46" s="6"/>
       <c r="AI46" s="6"/>
       <c r="BO46" s="6"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="L47" s="8"/>
       <c r="AG47" s="6"/>
       <c r="AH47" s="6"/>
       <c r="AI47" s="6"/>
       <c r="BO47" s="6"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="L48" s="8"/>
       <c r="AG48" s="6"/>
       <c r="AH48" s="6"/>
       <c r="AI48" s="6"/>
@@ -1740,45 +1756,47 @@
       <c r="E49" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L49" s="7"/>
+      <c r="L49" s="8"/>
       <c r="AG49" s="6"/>
       <c r="AH49" s="6"/>
       <c r="AI49" s="6"/>
       <c r="BO49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="7"/>
+      <c r="L50" s="8"/>
       <c r="AG50" s="6"/>
       <c r="AH50" s="6"/>
       <c r="AI50" s="6"/>
       <c r="BO50" s="6"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L51" s="7"/>
+      <c r="C51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="L51" s="8"/>
       <c r="AG51" s="6"/>
       <c r="AH51" s="6"/>
       <c r="AI51" s="6"/>
@@ -1800,86 +1818,89 @@
       <c r="E52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L52" s="7"/>
+      <c r="L52" s="8"/>
       <c r="AG52" s="6"/>
       <c r="AH52" s="6"/>
       <c r="AI52" s="6"/>
       <c r="BO52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L53" s="7"/>
+      <c r="C53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="L53" s="8"/>
       <c r="AG53" s="6"/>
       <c r="AH53" s="6"/>
       <c r="AI53" s="6"/>
       <c r="BO53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L54" s="7"/>
+      <c r="C54" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="7"/>
+      <c r="L54" s="8"/>
       <c r="AG54" s="6"/>
       <c r="AH54" s="6"/>
       <c r="AI54" s="6"/>
       <c r="BO54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="D55" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L55" s="7"/>
+      <c r="L55" s="8"/>
       <c r="AG55" s="6"/>
       <c r="AH55" s="6"/>
       <c r="AI55" s="6"/>
       <c r="BO55" s="6"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L56" s="7"/>
+      <c r="C56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="7"/>
+      <c r="L56" s="8"/>
       <c r="AG56" s="6"/>
       <c r="AH56" s="6"/>
       <c r="AI56" s="6"/>
@@ -1901,26 +1922,27 @@
       <c r="E57" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="L57" s="7"/>
+      <c r="L57" s="8"/>
       <c r="AG57" s="6"/>
       <c r="AH57" s="6"/>
       <c r="AI57" s="6"/>
       <c r="BO57" s="6"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L58" s="7"/>
+      <c r="D58" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="7"/>
+      <c r="L58" s="8"/>
       <c r="AG58" s="6"/>
       <c r="AH58" s="6"/>
       <c r="AI58" s="6"/>
@@ -1942,51 +1964,51 @@
       <c r="E59" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L59" s="7"/>
+      <c r="L59" s="8"/>
       <c r="AG59" s="6"/>
       <c r="AH59" s="6"/>
       <c r="AI59" s="6"/>
       <c r="BO59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="D60" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="L60" s="7"/>
+      <c r="L60" s="8"/>
       <c r="AG60" s="6"/>
       <c r="AH60" s="6"/>
       <c r="AI60" s="6"/>
       <c r="BO60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="C61" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L61" s="7"/>
+      <c r="L61" s="8"/>
       <c r="AG61" s="6"/>
       <c r="AH61" s="6"/>
       <c r="AI61" s="6"/>
@@ -2008,73 +2030,73 @@
       <c r="E62" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L62" s="7"/>
+      <c r="L62" s="8"/>
       <c r="AG62" s="6"/>
       <c r="AH62" s="6"/>
       <c r="AI62" s="6"/>
       <c r="BO62" s="6"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="C63" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L63" s="7"/>
+      <c r="L63" s="8"/>
       <c r="AG63" s="6"/>
       <c r="AH63" s="6"/>
       <c r="AI63" s="6"/>
       <c r="BO63" s="6"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="1" t="s">
+      <c r="C64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L64" s="7"/>
+      <c r="L64" s="8"/>
       <c r="AG64" s="6"/>
       <c r="AH64" s="6"/>
       <c r="AI64" s="6"/>
       <c r="BO64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="C65" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L65" s="7"/>
+      <c r="L65" s="8"/>
       <c r="AG65" s="6"/>
       <c r="AH65" s="6"/>
       <c r="AI65" s="6"/>
@@ -2096,7 +2118,7 @@
       <c r="E66" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L66" s="7"/>
+      <c r="L66" s="8"/>
       <c r="AG66" s="6"/>
       <c r="AH66" s="6"/>
       <c r="AI66" s="6"/>
@@ -2118,542 +2140,542 @@
       <c r="E67" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L67" s="7"/>
+      <c r="L67" s="8"/>
       <c r="AG67" s="6"/>
       <c r="AH67" s="6"/>
       <c r="AI67" s="6"/>
       <c r="BO67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="1" t="s">
+      <c r="C68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L68" s="7"/>
+      <c r="L68" s="8"/>
       <c r="AG68" s="6"/>
       <c r="AH68" s="6"/>
       <c r="AI68" s="6"/>
       <c r="BO68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="1" t="s">
+      <c r="C69" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L69" s="7"/>
+      <c r="L69" s="8"/>
       <c r="AG69" s="6"/>
       <c r="AH69" s="6"/>
       <c r="AI69" s="6"/>
       <c r="BO69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="1" t="s">
+      <c r="C70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L70" s="7"/>
+      <c r="L70" s="8"/>
       <c r="AG70" s="6"/>
       <c r="AH70" s="6"/>
       <c r="AI70" s="6"/>
       <c r="BO70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="1" t="s">
+      <c r="C71" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L71" s="7"/>
+      <c r="L71" s="8"/>
       <c r="AG71" s="6"/>
       <c r="AH71" s="6"/>
       <c r="AI71" s="6"/>
       <c r="BO71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="C72" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L72" s="7"/>
+      <c r="L72" s="8"/>
       <c r="AG72" s="6"/>
       <c r="AH72" s="6"/>
       <c r="AI72" s="6"/>
       <c r="BO72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="1" t="s">
+      <c r="C73" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L73" s="7"/>
+      <c r="L73" s="8"/>
       <c r="AG73" s="6"/>
       <c r="AH73" s="6"/>
       <c r="AI73" s="6"/>
       <c r="BO73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" s="1" t="s">
+      <c r="C74" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L74" s="7"/>
+      <c r="L74" s="8"/>
       <c r="AG74" s="6"/>
       <c r="AH74" s="6"/>
       <c r="AI74" s="6"/>
       <c r="BO74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="1" t="s">
+      <c r="C75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L75" s="7"/>
+      <c r="L75" s="8"/>
       <c r="AG75" s="6"/>
       <c r="AH75" s="6"/>
       <c r="AI75" s="6"/>
       <c r="BO75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="1" t="s">
+      <c r="C76" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L76" s="7"/>
+      <c r="L76" s="8"/>
       <c r="AG76" s="6"/>
       <c r="AH76" s="6"/>
       <c r="AI76" s="6"/>
       <c r="BO76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="C77" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L77" s="7"/>
+      <c r="L77" s="8"/>
       <c r="AG77" s="6"/>
       <c r="AH77" s="6"/>
       <c r="AI77" s="6"/>
       <c r="BO77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L78" s="7"/>
+      <c r="L78" s="8"/>
       <c r="AG78" s="6"/>
       <c r="AH78" s="6"/>
       <c r="AI78" s="6"/>
       <c r="BO78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L79" s="7"/>
+      <c r="L79" s="8"/>
       <c r="AG79" s="6"/>
       <c r="AH79" s="6"/>
       <c r="AI79" s="6"/>
       <c r="BO79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L80" s="7"/>
+      <c r="L80" s="8"/>
       <c r="AG80" s="6"/>
       <c r="AH80" s="6"/>
       <c r="AI80" s="6"/>
       <c r="BO80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L81" s="7"/>
+      <c r="L81" s="8"/>
       <c r="AG81" s="6"/>
       <c r="AH81" s="6"/>
       <c r="AI81" s="6"/>
       <c r="BO81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L82" s="7"/>
+      <c r="L82" s="8"/>
       <c r="AG82" s="6"/>
       <c r="AH82" s="6"/>
       <c r="AI82" s="6"/>
       <c r="BO82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L83" s="7"/>
+      <c r="L83" s="8"/>
       <c r="AG83" s="6"/>
       <c r="AH83" s="6"/>
       <c r="AI83" s="6"/>
       <c r="BO83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L84" s="7"/>
+      <c r="L84" s="8"/>
       <c r="AG84" s="6"/>
       <c r="AH84" s="6"/>
       <c r="AI84" s="6"/>
       <c r="BO84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L85" s="7"/>
+      <c r="L85" s="8"/>
       <c r="AG85" s="6"/>
       <c r="AH85" s="6"/>
       <c r="AI85" s="6"/>
       <c r="BO85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L86" s="7"/>
+      <c r="L86" s="8"/>
       <c r="AG86" s="6"/>
       <c r="AH86" s="6"/>
       <c r="AI86" s="6"/>
       <c r="BO86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L87" s="7"/>
+      <c r="L87" s="8"/>
       <c r="AG87" s="6"/>
       <c r="AH87" s="6"/>
       <c r="AI87" s="6"/>
       <c r="BO87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L88" s="7"/>
+      <c r="L88" s="8"/>
       <c r="AG88" s="6"/>
       <c r="AH88" s="6"/>
       <c r="AI88" s="6"/>
       <c r="BO88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L89" s="7"/>
+      <c r="L89" s="8"/>
       <c r="AG89" s="6"/>
       <c r="AH89" s="6"/>
       <c r="AI89" s="6"/>
       <c r="BO89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L90" s="7"/>
+      <c r="L90" s="8"/>
       <c r="AG90" s="6"/>
       <c r="AH90" s="6"/>
       <c r="AI90" s="6"/>
       <c r="BO90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L91" s="7"/>
+      <c r="L91" s="8"/>
       <c r="AG91" s="6"/>
       <c r="AH91" s="6"/>
       <c r="AI91" s="6"/>
       <c r="BO91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L92" s="7"/>
+      <c r="L92" s="8"/>
       <c r="AG92" s="6"/>
       <c r="AH92" s="6"/>
       <c r="AI92" s="6"/>
       <c r="BO92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L93" s="7"/>
+      <c r="L93" s="8"/>
       <c r="AG93" s="6"/>
       <c r="AH93" s="6"/>
       <c r="AI93" s="6"/>
       <c r="BO93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L94" s="7"/>
+      <c r="L94" s="8"/>
       <c r="AG94" s="6"/>
       <c r="AH94" s="6"/>
       <c r="AI94" s="6"/>
       <c r="BO94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L95" s="7"/>
+      <c r="L95" s="8"/>
       <c r="AG95" s="6"/>
       <c r="AH95" s="6"/>
       <c r="AI95" s="6"/>
       <c r="BO95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L96" s="7"/>
+      <c r="L96" s="8"/>
       <c r="AG96" s="6"/>
       <c r="AH96" s="6"/>
       <c r="AI96" s="6"/>
       <c r="BO96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L97" s="7"/>
+      <c r="L97" s="8"/>
       <c r="AG97" s="6"/>
       <c r="AH97" s="6"/>
       <c r="AI97" s="6"/>
       <c r="BO97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L98" s="7"/>
+      <c r="L98" s="8"/>
       <c r="AG98" s="6"/>
       <c r="AH98" s="6"/>
       <c r="AI98" s="6"/>
       <c r="BO98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L99" s="7"/>
+      <c r="L99" s="8"/>
       <c r="AG99" s="6"/>
       <c r="AH99" s="6"/>
       <c r="AI99" s="6"/>
       <c r="BO99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L100" s="7"/>
+      <c r="L100" s="8"/>
       <c r="AG100" s="6"/>
       <c r="AH100" s="6"/>
       <c r="AI100" s="6"/>
       <c r="BO100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L101" s="7"/>
+      <c r="L101" s="8"/>
       <c r="AG101" s="6"/>
       <c r="AH101" s="6"/>
       <c r="AI101" s="6"/>
       <c r="BO101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L102" s="7"/>
+      <c r="L102" s="8"/>
       <c r="AG102" s="6"/>
       <c r="AH102" s="6"/>
       <c r="AI102" s="6"/>
       <c r="BO102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L103" s="7"/>
+      <c r="L103" s="8"/>
       <c r="AG103" s="6"/>
       <c r="AH103" s="6"/>
       <c r="AI103" s="6"/>
       <c r="BO103" s="6"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L104" s="7"/>
+      <c r="L104" s="8"/>
       <c r="AG104" s="6"/>
       <c r="AH104" s="6"/>
       <c r="AI104" s="6"/>
       <c r="BO104" s="6"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L105" s="7"/>
+      <c r="L105" s="8"/>
       <c r="AG105" s="6"/>
       <c r="AH105" s="6"/>
       <c r="AI105" s="6"/>
       <c r="BO105" s="6"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L106" s="7"/>
+      <c r="L106" s="8"/>
       <c r="AG106" s="6"/>
       <c r="AH106" s="6"/>
       <c r="AI106" s="6"/>
       <c r="BO106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L107" s="7"/>
+      <c r="L107" s="8"/>
       <c r="AG107" s="6"/>
       <c r="AH107" s="6"/>
       <c r="AI107" s="6"/>
       <c r="BO107" s="6"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L108" s="7"/>
+      <c r="L108" s="8"/>
       <c r="AG108" s="6"/>
       <c r="AH108" s="6"/>
       <c r="AI108" s="6"/>
       <c r="BO108" s="6"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L109" s="7"/>
+      <c r="L109" s="8"/>
       <c r="AG109" s="6"/>
       <c r="AH109" s="6"/>
       <c r="AI109" s="6"/>
       <c r="BO109" s="6"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L110" s="7"/>
+      <c r="L110" s="8"/>
       <c r="AG110" s="6"/>
       <c r="AH110" s="6"/>
       <c r="AI110" s="6"/>
       <c r="BO110" s="6"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L111" s="7"/>
+      <c r="L111" s="8"/>
       <c r="AG111" s="6"/>
       <c r="AH111" s="6"/>
       <c r="AI111" s="6"/>
       <c r="BO111" s="6"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L112" s="7"/>
+      <c r="L112" s="8"/>
       <c r="AG112" s="6"/>
       <c r="AH112" s="6"/>
       <c r="AI112" s="6"/>
       <c r="BO112" s="6"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L113" s="7"/>
+      <c r="L113" s="8"/>
       <c r="AG113" s="6"/>
       <c r="AH113" s="6"/>
       <c r="AI113" s="6"/>
       <c r="BO113" s="6"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L114" s="7"/>
+      <c r="L114" s="8"/>
       <c r="AG114" s="6"/>
       <c r="AH114" s="6"/>
       <c r="AI114" s="6"/>
       <c r="BO114" s="6"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L115" s="7"/>
+      <c r="L115" s="8"/>
       <c r="AG115" s="6"/>
       <c r="AH115" s="6"/>
       <c r="AI115" s="6"/>
       <c r="BO115" s="6"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L116" s="7"/>
+      <c r="L116" s="8"/>
       <c r="AG116" s="6"/>
       <c r="AH116" s="6"/>
       <c r="AI116" s="6"/>
       <c r="BO116" s="6"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L117" s="7"/>
+      <c r="L117" s="8"/>
       <c r="AG117" s="6"/>
       <c r="AH117" s="6"/>
       <c r="AI117" s="6"/>
       <c r="BO117" s="6"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L118" s="7"/>
+      <c r="L118" s="8"/>
       <c r="AG118" s="6"/>
       <c r="AH118" s="6"/>
       <c r="AI118" s="6"/>
       <c r="BO118" s="6"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L119" s="7"/>
+      <c r="L119" s="8"/>
       <c r="AG119" s="6"/>
       <c r="AH119" s="6"/>
       <c r="AI119" s="6"/>
       <c r="BO119" s="6"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L120" s="7"/>
+      <c r="L120" s="8"/>
       <c r="AG120" s="6"/>
       <c r="AH120" s="6"/>
       <c r="AI120" s="6"/>
       <c r="BO120" s="6"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L121" s="7"/>
+      <c r="L121" s="8"/>
       <c r="AG121" s="6"/>
       <c r="AH121" s="6"/>
       <c r="AI121" s="6"/>
       <c r="BO121" s="6"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L122" s="7"/>
+      <c r="L122" s="8"/>
       <c r="AG122" s="6"/>
       <c r="AH122" s="6"/>
       <c r="AI122" s="6"/>

</xml_diff>

<commit_message>
full initial analisis and dataset reduction
</commit_message>
<xml_diff>
--- a/data/seera_analysis.xlsx
+++ b/data/seera_analysis.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="119">
   <si>
     <t xml:space="preserve">Group</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t xml:space="preserve">DBMS used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5? 4 categories</t>
   </si>
   <si>
     <t xml:space="preserve">Technical stability</t>
@@ -622,8 +625,8 @@
   </sheetPr>
   <dimension ref="A1:BO122"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1941,7 +1944,9 @@
       <c r="D58" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="7"/>
+      <c r="E58" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="L58" s="8"/>
       <c r="AG58" s="6"/>
       <c r="AH58" s="6"/>
@@ -1953,7 +1958,7 @@
         <v>88</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>7</v>
@@ -1975,7 +1980,7 @@
         <v>88</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>73</v>
@@ -1997,7 +2002,7 @@
         <v>88</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>7</v>
@@ -2019,7 +2024,7 @@
         <v>88</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>7</v>
@@ -2028,7 +2033,7 @@
         <v>8</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L62" s="8"/>
       <c r="AG62" s="6"/>
@@ -2041,7 +2046,7 @@
         <v>88</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>7</v>
@@ -2063,7 +2068,7 @@
         <v>88</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>7</v>
@@ -2085,7 +2090,7 @@
         <v>88</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>7</v>
@@ -2107,7 +2112,7 @@
         <v>88</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>7</v>
@@ -2129,7 +2134,7 @@
         <v>88</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>27</v>
@@ -2148,10 +2153,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>7</v>
@@ -2170,10 +2175,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>7</v>
@@ -2192,10 +2197,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>7</v>
@@ -2214,10 +2219,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>7</v>
@@ -2236,10 +2241,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>7</v>
@@ -2258,10 +2263,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>7</v>
@@ -2280,10 +2285,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>7</v>
@@ -2302,10 +2307,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>7</v>
@@ -2324,10 +2329,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>7</v>
@@ -2346,10 +2351,10 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>7</v>

</xml_diff>